<commit_message>
Updated MEX model - 2025-07-28 18:36
</commit_message>
<xml_diff>
--- a/VerveStacks_MEX/SuppXLS/Scen_Par-NGFS.xlsx
+++ b/VerveStacks_MEX/SuppXLS/Scen_Par-NGFS.xlsx
@@ -5,17 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\VerveStacks\assumptions\VerveStacks_ISO_template\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_MEX\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B9825A8-41F6-43CC-881C-60AA24444A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2284A2D-8690-48E1-B18F-3FC3B3E1F994}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Veda" sheetId="1" r:id="rId1"/>
-    <sheet name="iamc_data" sheetId="2" r:id="rId2"/>
-    <sheet name="base_year_data" sheetId="3" r:id="rId3"/>
+    <sheet name="historical_data" sheetId="4" r:id="rId1"/>
+    <sheet name="Veda" sheetId="1" r:id="rId2"/>
+    <sheet name="iamc_data" sheetId="2" r:id="rId3"/>
+    <sheet name="base_year_data" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="454" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="55">
   <si>
     <t>~Inputcell: 3</t>
   </si>
@@ -95,27 +96,6 @@
   </si>
   <si>
     <t>Unit</t>
-  </si>
-  <si>
-    <t>2020</t>
-  </si>
-  <si>
-    <t>2025</t>
-  </si>
-  <si>
-    <t>2030</t>
-  </si>
-  <si>
-    <t>2035</t>
-  </si>
-  <si>
-    <t>2040</t>
-  </si>
-  <si>
-    <t>2045</t>
-  </si>
-  <si>
-    <t>2050</t>
   </si>
   <si>
     <t>variable</t>
@@ -699,10 +679,274 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2BC4618-DE5A-4601-8D55-FC829A84DBEA}">
+  <dimension ref="A1:H10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2">
+        <v>0.7</v>
+      </c>
+      <c r="D2">
+        <v>2.4</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>6.7</v>
+      </c>
+      <c r="G2">
+        <v>0.26</v>
+      </c>
+      <c r="H2">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3">
+        <v>21.5</v>
+      </c>
+      <c r="D3">
+        <v>21.4</v>
+      </c>
+      <c r="E3">
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <v>21.4</v>
+      </c>
+      <c r="G3">
+        <v>0.46</v>
+      </c>
+      <c r="H3">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>257.3</v>
+      </c>
+      <c r="D4">
+        <v>192.6</v>
+      </c>
+      <c r="E4">
+        <v>217.5</v>
+      </c>
+      <c r="F4">
+        <v>192.1</v>
+      </c>
+      <c r="G4">
+        <v>0.67</v>
+      </c>
+      <c r="H4">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5">
+        <v>4.3</v>
+      </c>
+      <c r="E5">
+        <v>4.5</v>
+      </c>
+      <c r="G5">
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6">
+        <v>33</v>
+      </c>
+      <c r="D6">
+        <v>31.6</v>
+      </c>
+      <c r="E6">
+        <v>35.9</v>
+      </c>
+      <c r="F6">
+        <v>35.6</v>
+      </c>
+      <c r="G6">
+        <v>0.32</v>
+      </c>
+      <c r="H6">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>10.8</v>
+      </c>
+      <c r="D7">
+        <v>10.8</v>
+      </c>
+      <c r="E7">
+        <v>10.9</v>
+      </c>
+      <c r="F7">
+        <v>10.9</v>
+      </c>
+      <c r="G7">
+        <v>0.77</v>
+      </c>
+      <c r="H7">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8">
+        <v>6.7</v>
+      </c>
+      <c r="D8">
+        <v>8.4</v>
+      </c>
+      <c r="E8">
+        <v>39.799999999999997</v>
+      </c>
+      <c r="F8">
+        <v>32.700000000000003</v>
+      </c>
+      <c r="G8">
+        <v>0.11</v>
+      </c>
+      <c r="H8">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9">
+        <v>28.2</v>
+      </c>
+      <c r="D9">
+        <v>27.9</v>
+      </c>
+      <c r="E9">
+        <v>20.6</v>
+      </c>
+      <c r="F9">
+        <v>20.3</v>
+      </c>
+      <c r="G9">
+        <v>0.25</v>
+      </c>
+      <c r="H9">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10">
+        <v>22.3</v>
+      </c>
+      <c r="D10">
+        <v>23.1</v>
+      </c>
+      <c r="E10">
+        <v>20.6</v>
+      </c>
+      <c r="F10">
+        <v>20.5</v>
+      </c>
+      <c r="G10">
+        <v>0.31</v>
+      </c>
+      <c r="H10">
+        <v>0.32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:AA19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R11" sqref="R11"/>
     </sheetView>
   </sheetViews>
@@ -769,7 +1013,7 @@
         <v>340.2</v>
       </c>
       <c r="R10" s="4" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="2:27" ht="14.65" thickTop="1" x14ac:dyDescent="0.45">
@@ -802,31 +1046,31 @@
       </c>
     </row>
     <row r="15" spans="2:27" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="G15" t="str">
+      <c r="G15">
         <f>iamc_data!F1</f>
         <v>2020</v>
       </c>
-      <c r="H15" t="str">
+      <c r="H15">
         <f>iamc_data!G1</f>
         <v>2025</v>
       </c>
-      <c r="I15" t="str">
+      <c r="I15">
         <f>iamc_data!H1</f>
         <v>2030</v>
       </c>
-      <c r="J15" t="str">
+      <c r="J15">
         <f>iamc_data!I1</f>
         <v>2035</v>
       </c>
-      <c r="K15" t="str">
+      <c r="K15">
         <f>iamc_data!J1</f>
         <v>2040</v>
       </c>
-      <c r="L15" t="str">
+      <c r="L15">
         <f>iamc_data!K1</f>
         <v>2045</v>
       </c>
-      <c r="M15" t="str">
+      <c r="M15">
         <f>iamc_data!L1</f>
         <v>2050</v>
       </c>
@@ -922,7 +1166,7 @@
         <v>12</v>
       </c>
       <c r="AA16" s="4" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="7:25" x14ac:dyDescent="0.45">
@@ -962,7 +1206,7 @@
         <v>175.33862002360769</v>
       </c>
       <c r="S17" s="1">
-        <f t="shared" ref="S16:X18" si="1">R17*H17/G17</f>
+        <f t="shared" ref="S17:X18" si="1">R17*H17/G17</f>
         <v>220.67915012340382</v>
       </c>
       <c r="T17" s="1">
@@ -1055,7 +1299,7 @@
     </row>
     <row r="19" spans="7:25" x14ac:dyDescent="0.45">
       <c r="Q19" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="R19" s="1">
         <f>$Q$10*G16/SUM($G$16:$G$18)-R16</f>
@@ -1094,7 +1338,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O50"/>
   <sheetViews>
@@ -1103,67 +1347,67 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.45">
-      <c r="A1" s="3" t="s">
+      <c r="A1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1">
+        <v>2020</v>
+      </c>
+      <c r="G1">
+        <v>2025</v>
+      </c>
+      <c r="H1">
+        <v>2030</v>
+      </c>
+      <c r="I1">
+        <v>2035</v>
+      </c>
+      <c r="J1">
+        <v>2040</v>
+      </c>
+      <c r="K1">
+        <v>2045</v>
+      </c>
+      <c r="L1">
+        <v>2050</v>
+      </c>
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="N1" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F2">
         <v>0.47449999999999998</v>
@@ -1187,10 +1431,10 @@
         <v>0.34499999999999997</v>
       </c>
       <c r="M2" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="N2" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O2" t="s">
         <v>14</v>
@@ -1198,19 +1442,19 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F3">
         <v>0.45100000000000001</v>
@@ -1234,10 +1478,10 @@
         <v>1.149</v>
       </c>
       <c r="M3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="N3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O3" t="s">
         <v>14</v>
@@ -1245,19 +1489,19 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F4">
         <v>3.0999999999999999E-3</v>
@@ -1281,10 +1525,10 @@
         <v>0.42399999999999999</v>
       </c>
       <c r="M4" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="N4" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O4" t="s">
         <v>11</v>
@@ -1292,19 +1536,19 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F5">
         <v>0.4803</v>
@@ -1328,10 +1572,10 @@
         <v>1.3394999999999999</v>
       </c>
       <c r="M5" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="N5" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O5" t="s">
         <v>13</v>
@@ -1339,19 +1583,19 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F6">
         <v>0.44850000000000001</v>
@@ -1375,10 +1619,10 @@
         <v>0.15759999999999999</v>
       </c>
       <c r="M6" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="N6" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O6" t="s">
         <v>14</v>
@@ -1386,19 +1630,19 @@
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F7">
         <v>0.44600000000000001</v>
@@ -1422,10 +1666,10 @@
         <v>0.2162</v>
       </c>
       <c r="M7" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="N7" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O7" t="s">
         <v>14</v>
@@ -1433,19 +1677,19 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F8">
         <v>0.47439999999999999</v>
@@ -1469,10 +1713,10 @@
         <v>1.6169</v>
       </c>
       <c r="M8" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="N8" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O8" t="s">
         <v>13</v>
@@ -1480,19 +1724,19 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F9">
         <v>2.8999999999999998E-3</v>
@@ -1516,10 +1760,10 @@
         <v>0.79069999999999996</v>
       </c>
       <c r="M9" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="N9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O9" t="s">
         <v>11</v>
@@ -1527,19 +1771,19 @@
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F10">
         <v>1.8E-3</v>
@@ -1563,10 +1807,10 @@
         <v>0.24879999999999999</v>
       </c>
       <c r="M10" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="N10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O10" t="s">
         <v>11</v>
@@ -1574,19 +1818,19 @@
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F11">
         <v>0.49619999999999997</v>
@@ -1610,10 +1854,10 @@
         <v>1.6558999999999999</v>
       </c>
       <c r="M11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="N11" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O11" t="s">
         <v>13</v>
@@ -1621,19 +1865,19 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F12">
         <v>0.47139999999999999</v>
@@ -1657,10 +1901,10 @@
         <v>0.18659999999999999</v>
       </c>
       <c r="M12" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="N12" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O12" t="s">
         <v>14</v>
@@ -1668,19 +1912,19 @@
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F13">
         <v>0.47810000000000002</v>
@@ -1704,10 +1948,10 @@
         <v>1.4411</v>
       </c>
       <c r="M13" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="N13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O13" t="s">
         <v>13</v>
@@ -1715,19 +1959,19 @@
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F14">
         <v>3.3999999999999998E-3</v>
@@ -1751,10 +1995,10 @@
         <v>0.72319999999999995</v>
       </c>
       <c r="M14" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="N14" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O14" t="s">
         <v>11</v>
@@ -1762,19 +2006,19 @@
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F15">
         <v>0.47349999999999998</v>
@@ -1798,10 +2042,10 @@
         <v>1.673</v>
       </c>
       <c r="M15" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="N15" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O15" t="s">
         <v>13</v>
@@ -1809,19 +2053,19 @@
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F16">
         <v>0.44269999999999998</v>
@@ -1845,10 +2089,10 @@
         <v>0.47089999999999999</v>
       </c>
       <c r="M16" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="N16" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O16" t="s">
         <v>14</v>
@@ -1856,19 +2100,19 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F17">
         <v>3.0000000000000001E-3</v>
@@ -1892,10 +2136,10 @@
         <v>0.55869999999999997</v>
       </c>
       <c r="M17" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="N17" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O17" t="s">
         <v>11</v>
@@ -1903,19 +2147,19 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F18">
         <v>0.47439999999999999</v>
@@ -1939,10 +2183,10 @@
         <v>1.6732</v>
       </c>
       <c r="M18" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="N18" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O18" t="s">
         <v>13</v>
@@ -1950,19 +2194,19 @@
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B19" t="s">
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F19">
         <v>0.45379999999999998</v>
@@ -1986,10 +2230,10 @@
         <v>0.254</v>
       </c>
       <c r="M19" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="N19" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O19" t="s">
         <v>14</v>
@@ -1997,19 +2241,19 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B20" t="s">
         <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D20" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F20">
         <v>0.46850000000000003</v>
@@ -2033,10 +2277,10 @@
         <v>0.68589999999999995</v>
       </c>
       <c r="M20" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="N20" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O20" t="s">
         <v>13</v>
@@ -2044,19 +2288,19 @@
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B21" t="s">
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F21">
         <v>2.8999999999999998E-3</v>
@@ -2080,10 +2324,10 @@
         <v>0.54420000000000002</v>
       </c>
       <c r="M21" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="N21" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O21" t="s">
         <v>11</v>
@@ -2091,19 +2335,19 @@
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="F22">
         <v>1.6999999999999999E-3</v>
@@ -2127,10 +2371,10 @@
         <v>0.60589999999999999</v>
       </c>
       <c r="M22" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="N22" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="O22" t="s">
         <v>11</v>
@@ -2138,19 +2382,19 @@
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
       </c>
       <c r="C23" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
         <v>30</v>
-      </c>
-      <c r="D23" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" t="s">
-        <v>37</v>
       </c>
       <c r="F23">
         <v>0</v>
@@ -2174,30 +2418,30 @@
         <v>40.9756</v>
       </c>
       <c r="M23" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="N23" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O23" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>2</v>
       </c>
       <c r="C24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" t="s">
         <v>30</v>
-      </c>
-      <c r="D24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" t="s">
-        <v>37</v>
       </c>
       <c r="F24">
         <v>1.6883999999999999</v>
@@ -2221,30 +2465,30 @@
         <v>8.3480000000000008</v>
       </c>
       <c r="M24" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="N24" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O24" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
       </c>
       <c r="C25" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" t="s">
+        <v>35</v>
+      </c>
+      <c r="E25" t="s">
         <v>30</v>
-      </c>
-      <c r="D25" t="s">
-        <v>42</v>
-      </c>
-      <c r="E25" t="s">
-        <v>37</v>
       </c>
       <c r="F25">
         <v>1.8954</v>
@@ -2268,30 +2512,30 @@
         <v>7.8837999999999999</v>
       </c>
       <c r="M25" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N25" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O25" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B26" t="s">
         <v>4</v>
       </c>
       <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>35</v>
+      </c>
+      <c r="E26" t="s">
         <v>30</v>
-      </c>
-      <c r="D26" t="s">
-        <v>42</v>
-      </c>
-      <c r="E26" t="s">
-        <v>37</v>
       </c>
       <c r="F26">
         <v>1.8954</v>
@@ -2315,30 +2559,30 @@
         <v>4.4329000000000001</v>
       </c>
       <c r="M26" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N26" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O26" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B27" t="s">
         <v>6</v>
       </c>
       <c r="C27" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" t="s">
+        <v>33</v>
+      </c>
+      <c r="E27" t="s">
         <v>30</v>
-      </c>
-      <c r="D27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E27" t="s">
-        <v>37</v>
       </c>
       <c r="F27">
         <v>1.6883999999999999</v>
@@ -2362,30 +2606,30 @@
         <v>4.5853999999999999</v>
       </c>
       <c r="M27" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="N27" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O27" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B28" t="s">
         <v>4</v>
       </c>
       <c r="C28" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" t="s">
         <v>30</v>
-      </c>
-      <c r="D28" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" t="s">
-        <v>37</v>
       </c>
       <c r="F28">
         <v>3.1419999999999999</v>
@@ -2409,30 +2653,30 @@
         <v>4.5537999999999998</v>
       </c>
       <c r="M28" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="N28" t="s">
+        <v>31</v>
+      </c>
+      <c r="O28" t="s">
         <v>38</v>
-      </c>
-      <c r="O28" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B29" t="s">
         <v>4</v>
       </c>
       <c r="C29" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+      <c r="E29" t="s">
         <v>30</v>
-      </c>
-      <c r="D29" t="s">
-        <v>36</v>
-      </c>
-      <c r="E29" t="s">
-        <v>37</v>
       </c>
       <c r="F29">
         <v>0</v>
@@ -2456,30 +2700,30 @@
         <v>8.2246000000000006</v>
       </c>
       <c r="M29" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="N29" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O29" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B30" t="s">
         <v>4</v>
       </c>
       <c r="C30" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" t="s">
+        <v>33</v>
+      </c>
+      <c r="E30" t="s">
         <v>30</v>
-      </c>
-      <c r="D30" t="s">
-        <v>40</v>
-      </c>
-      <c r="E30" t="s">
-        <v>37</v>
       </c>
       <c r="F30">
         <v>1.6883999999999999</v>
@@ -2503,30 +2747,30 @@
         <v>3.1934999999999998</v>
       </c>
       <c r="M30" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="N30" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O30" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B31" t="s">
         <v>2</v>
       </c>
       <c r="C31" t="s">
+        <v>23</v>
+      </c>
+      <c r="D31" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" t="s">
         <v>30</v>
-      </c>
-      <c r="D31" t="s">
-        <v>44</v>
-      </c>
-      <c r="E31" t="s">
-        <v>37</v>
       </c>
       <c r="F31">
         <v>3.1419999999999999</v>
@@ -2550,30 +2794,30 @@
         <v>3.4415</v>
       </c>
       <c r="M31" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="N31" t="s">
+        <v>31</v>
+      </c>
+      <c r="O31" t="s">
         <v>38</v>
-      </c>
-      <c r="O31" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B32" t="s">
         <v>6</v>
       </c>
       <c r="C32" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" t="s">
         <v>30</v>
-      </c>
-      <c r="D32" t="s">
-        <v>36</v>
-      </c>
-      <c r="E32" t="s">
-        <v>37</v>
       </c>
       <c r="F32">
         <v>0</v>
@@ -2597,30 +2841,30 @@
         <v>18.199000000000002</v>
       </c>
       <c r="M32" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="N32" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O32" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B33" t="s">
         <v>3</v>
       </c>
       <c r="C33" t="s">
+        <v>23</v>
+      </c>
+      <c r="D33" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" t="s">
         <v>30</v>
-      </c>
-      <c r="D33" t="s">
-        <v>36</v>
-      </c>
-      <c r="E33" t="s">
-        <v>37</v>
       </c>
       <c r="F33">
         <v>0</v>
@@ -2644,30 +2888,30 @@
         <v>6.5091000000000001</v>
       </c>
       <c r="M33" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="N33" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O33" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B34" t="s">
         <v>3</v>
       </c>
       <c r="C34" t="s">
+        <v>23</v>
+      </c>
+      <c r="D34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" t="s">
         <v>30</v>
-      </c>
-      <c r="D34" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" t="s">
-        <v>37</v>
       </c>
       <c r="F34">
         <v>1.8954</v>
@@ -2691,30 +2935,30 @@
         <v>4.1519000000000004</v>
       </c>
       <c r="M34" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N34" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O34" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B35" t="s">
         <v>1</v>
       </c>
       <c r="C35" t="s">
+        <v>23</v>
+      </c>
+      <c r="D35" t="s">
+        <v>29</v>
+      </c>
+      <c r="E35" t="s">
         <v>30</v>
-      </c>
-      <c r="D35" t="s">
-        <v>36</v>
-      </c>
-      <c r="E35" t="s">
-        <v>37</v>
       </c>
       <c r="F35">
         <v>0</v>
@@ -2738,30 +2982,30 @@
         <v>10.735799999999999</v>
       </c>
       <c r="M35" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="N35" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O35" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B36" t="s">
         <v>1</v>
       </c>
       <c r="C36" t="s">
+        <v>23</v>
+      </c>
+      <c r="D36" t="s">
+        <v>33</v>
+      </c>
+      <c r="E36" t="s">
         <v>30</v>
-      </c>
-      <c r="D36" t="s">
-        <v>40</v>
-      </c>
-      <c r="E36" t="s">
-        <v>37</v>
       </c>
       <c r="F36">
         <v>1.6883999999999999</v>
@@ -2785,30 +3029,30 @@
         <v>4.2481999999999998</v>
       </c>
       <c r="M36" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="N36" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O36" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B37" t="s">
         <v>1</v>
       </c>
       <c r="C37" t="s">
+        <v>23</v>
+      </c>
+      <c r="D37" t="s">
+        <v>35</v>
+      </c>
+      <c r="E37" t="s">
         <v>30</v>
-      </c>
-      <c r="D37" t="s">
-        <v>42</v>
-      </c>
-      <c r="E37" t="s">
-        <v>37</v>
       </c>
       <c r="F37">
         <v>1.8954</v>
@@ -2832,30 +3076,30 @@
         <v>4.4630000000000001</v>
       </c>
       <c r="M37" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N37" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O37" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
         <v>1</v>
       </c>
       <c r="C38" t="s">
+        <v>23</v>
+      </c>
+      <c r="D38" t="s">
+        <v>37</v>
+      </c>
+      <c r="E38" t="s">
         <v>30</v>
-      </c>
-      <c r="D38" t="s">
-        <v>44</v>
-      </c>
-      <c r="E38" t="s">
-        <v>37</v>
       </c>
       <c r="F38">
         <v>3.1419999999999999</v>
@@ -2879,30 +3123,30 @@
         <v>5.1703000000000001</v>
       </c>
       <c r="M38" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="N38" t="s">
+        <v>31</v>
+      </c>
+      <c r="O38" t="s">
         <v>38</v>
-      </c>
-      <c r="O38" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
       </c>
       <c r="C39" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" t="s">
+        <v>29</v>
+      </c>
+      <c r="E39" t="s">
         <v>30</v>
-      </c>
-      <c r="D39" t="s">
-        <v>36</v>
-      </c>
-      <c r="E39" t="s">
-        <v>37</v>
       </c>
       <c r="F39">
         <v>0</v>
@@ -2926,30 +3170,30 @@
         <v>14.2902</v>
       </c>
       <c r="M39" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="N39" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O39" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
       </c>
       <c r="C40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D40" t="s">
+        <v>33</v>
+      </c>
+      <c r="E40" t="s">
         <v>30</v>
-      </c>
-      <c r="D40" t="s">
-        <v>40</v>
-      </c>
-      <c r="E40" t="s">
-        <v>37</v>
       </c>
       <c r="F40">
         <v>1.6883999999999999</v>
@@ -2973,30 +3217,30 @@
         <v>6.0046999999999997</v>
       </c>
       <c r="M40" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="N40" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O40" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B41" t="s">
         <v>3</v>
       </c>
       <c r="C41" t="s">
+        <v>23</v>
+      </c>
+      <c r="D41" t="s">
+        <v>37</v>
+      </c>
+      <c r="E41" t="s">
         <v>30</v>
-      </c>
-      <c r="D41" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" t="s">
-        <v>37</v>
       </c>
       <c r="F41">
         <v>3.1419999999999999</v>
@@ -3020,30 +3264,30 @@
         <v>5.3041999999999998</v>
       </c>
       <c r="M41" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="N41" t="s">
+        <v>31</v>
+      </c>
+      <c r="O41" t="s">
         <v>38</v>
-      </c>
-      <c r="O41" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
       </c>
       <c r="C42" t="s">
+        <v>23</v>
+      </c>
+      <c r="D42" t="s">
+        <v>35</v>
+      </c>
+      <c r="E42" t="s">
         <v>30</v>
-      </c>
-      <c r="D42" t="s">
-        <v>42</v>
-      </c>
-      <c r="E42" t="s">
-        <v>37</v>
       </c>
       <c r="F42">
         <v>1.8954</v>
@@ -3067,30 +3311,30 @@
         <v>5.1092000000000004</v>
       </c>
       <c r="M42" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N42" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O42" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B43" t="s">
         <v>5</v>
       </c>
       <c r="C43" t="s">
+        <v>23</v>
+      </c>
+      <c r="D43" t="s">
+        <v>29</v>
+      </c>
+      <c r="E43" t="s">
         <v>30</v>
-      </c>
-      <c r="D43" t="s">
-        <v>36</v>
-      </c>
-      <c r="E43" t="s">
-        <v>37</v>
       </c>
       <c r="F43">
         <v>0</v>
@@ -3114,30 +3358,30 @@
         <v>3.1745000000000001</v>
       </c>
       <c r="M43" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="N43" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O43" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B44" t="s">
         <v>5</v>
       </c>
       <c r="C44" t="s">
+        <v>23</v>
+      </c>
+      <c r="D44" t="s">
+        <v>33</v>
+      </c>
+      <c r="E44" t="s">
         <v>30</v>
-      </c>
-      <c r="D44" t="s">
-        <v>40</v>
-      </c>
-      <c r="E44" t="s">
-        <v>37</v>
       </c>
       <c r="F44">
         <v>1.6883999999999999</v>
@@ -3161,30 +3405,30 @@
         <v>2.7404000000000002</v>
       </c>
       <c r="M44" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="N44" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O44" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B45" t="s">
         <v>5</v>
       </c>
       <c r="C45" t="s">
+        <v>23</v>
+      </c>
+      <c r="D45" t="s">
+        <v>35</v>
+      </c>
+      <c r="E45" t="s">
         <v>30</v>
-      </c>
-      <c r="D45" t="s">
-        <v>42</v>
-      </c>
-      <c r="E45" t="s">
-        <v>37</v>
       </c>
       <c r="F45">
         <v>1.8954</v>
@@ -3208,30 +3452,30 @@
         <v>4.0777999999999999</v>
       </c>
       <c r="M45" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N45" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O45" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B46" t="s">
         <v>5</v>
       </c>
       <c r="C46" t="s">
+        <v>23</v>
+      </c>
+      <c r="D46" t="s">
+        <v>37</v>
+      </c>
+      <c r="E46" t="s">
         <v>30</v>
-      </c>
-      <c r="D46" t="s">
-        <v>44</v>
-      </c>
-      <c r="E46" t="s">
-        <v>37</v>
       </c>
       <c r="F46">
         <v>3.1419999999999999</v>
@@ -3255,30 +3499,30 @@
         <v>5.5926</v>
       </c>
       <c r="M46" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="N46" t="s">
+        <v>31</v>
+      </c>
+      <c r="O46" t="s">
         <v>38</v>
-      </c>
-      <c r="O46" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B47" t="s">
         <v>6</v>
       </c>
       <c r="C47" t="s">
+        <v>23</v>
+      </c>
+      <c r="D47" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47" t="s">
         <v>30</v>
-      </c>
-      <c r="D47" t="s">
-        <v>42</v>
-      </c>
-      <c r="E47" t="s">
-        <v>37</v>
       </c>
       <c r="F47">
         <v>1.8954</v>
@@ -3302,30 +3546,30 @@
         <v>4.8287000000000004</v>
       </c>
       <c r="M47" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="N47" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O47" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
+        <v>23</v>
+      </c>
+      <c r="D48" t="s">
+        <v>33</v>
+      </c>
+      <c r="E48" t="s">
         <v>30</v>
-      </c>
-      <c r="D48" t="s">
-        <v>40</v>
-      </c>
-      <c r="E48" t="s">
-        <v>37</v>
       </c>
       <c r="F48">
         <v>1.6883999999999999</v>
@@ -3349,30 +3593,30 @@
         <v>2.9908999999999999</v>
       </c>
       <c r="M48" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="N48" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="O48" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B49" t="s">
         <v>7</v>
       </c>
       <c r="C49" t="s">
+        <v>23</v>
+      </c>
+      <c r="D49" t="s">
+        <v>37</v>
+      </c>
+      <c r="E49" t="s">
         <v>30</v>
-      </c>
-      <c r="D49" t="s">
-        <v>44</v>
-      </c>
-      <c r="E49" t="s">
-        <v>37</v>
       </c>
       <c r="F49">
         <v>3.1419999999999999</v>
@@ -3396,30 +3640,30 @@
         <v>6.3582999999999998</v>
       </c>
       <c r="M49" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="N49" t="s">
+        <v>31</v>
+      </c>
+      <c r="O49" t="s">
         <v>38</v>
-      </c>
-      <c r="O49" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B50" t="s">
         <v>6</v>
       </c>
       <c r="C50" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" t="s">
+        <v>37</v>
+      </c>
+      <c r="E50" t="s">
         <v>30</v>
-      </c>
-      <c r="D50" t="s">
-        <v>44</v>
-      </c>
-      <c r="E50" t="s">
-        <v>37</v>
       </c>
       <c r="F50">
         <v>3.1419999999999999</v>
@@ -3443,13 +3687,13 @@
         <v>2.6377999999999999</v>
       </c>
       <c r="M50" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="N50" t="s">
+        <v>31</v>
+      </c>
+      <c r="O50" t="s">
         <v>38</v>
-      </c>
-      <c r="O50" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3457,7 +3701,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H10"/>
   <sheetViews>
@@ -3478,36 +3722,36 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="C2">
         <v>0.7</v>
@@ -3530,10 +3774,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C3">
         <v>21.5</v>
@@ -3556,10 +3800,10 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C4">
         <v>257.3</v>
@@ -3582,10 +3826,10 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="C5">
         <v>4.3</v>
@@ -3599,10 +3843,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C6">
         <v>33</v>
@@ -3625,10 +3869,10 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B7" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C7">
         <v>10.8</v>
@@ -3651,10 +3895,10 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="C8">
         <v>6.7</v>
@@ -3677,10 +3921,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C9">
         <v>28.2</v>
@@ -3703,10 +3947,10 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C10">
         <v>22.3</v>

</xml_diff>